<commit_message>
File Containing Website URLs
</commit_message>
<xml_diff>
--- a/sample_data/file.xlsx
+++ b/sample_data/file.xlsx
@@ -1,33 +1,54 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\My_Project\sample_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Attack URL</t>
+  </si>
+  <si>
+    <t>Context</t>
+  </si>
+  <si>
+    <t>Detection</t>
+  </si>
+  <si>
+    <t>Successful</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,12 +67,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -317,197 +347,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="109.7109375" customWidth="1" min="1" max="1"/>
-    <col width="18.140625" customWidth="1" min="2" max="2"/>
-    <col width="96.42578125" customWidth="1" min="3" max="3"/>
+    <col min="1" max="1" width="109.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="96.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Attack URL</t>
-        </is>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Context</t>
-        </is>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Detection</t>
-        </is>
+      <c r="C1" t="s">
+        <v>3</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>https://www.faz.net/suche/?query=' onmouseover='alert(1)&amp;resultsPerPage=20</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>ATTR</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>&lt;div class="js-adobe-digital-data is-Invisible" data-digital-data='{"site":{"digitalAsset":"faz.net"},"internalSearch":{"term":"' onmouseover='alert(1)","numberOfResults":0},"page":{"name":"2.2064","ressort":"Suche","type":"suche","title":"Suche","seoTitle":"Suche und Suchergebnisse - FAZ"}}'&gt;</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>https://www.cgiar.org?s=" onmouseover="alert(1)</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ATTR</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>&lt;input class=""
-               type="text"
-               name="s"
-               id="s"
-               value="" onmouseover="alert(1)"
-               placeholder="Enter a word" /&gt;</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>https://www.redrivercatalog.com/search.html?addsearch=' onmouseover='alert(1)</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>ATTR</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>&lt;input type="search" class="form-control" placeholder="Search" aria-label="search" aria-describedby="search" name="addsearch" value="' onmouseover='alert(1)"&gt;</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>https://www.zentechnologies.com/search/search.php?query=" onmouseover="alert(1)&amp;search=1</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>ATTR</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>&lt;input type="hidden" name="query" value="" onmouseover="alert(1)"&gt;</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>https://www.britannica.com/search?query=" onmouseover="alert(1)</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>ATTR</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>&lt;input name="query" id="search-page-search-query" placeholder="Search Britannica..." class="form-control form-control-lg search-query pr-50 shadow-sm" value="" onmouseover="alert(1)" maxlength="200" autocomplete="off"  aria-label="Search Britannica" /&gt;</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>https://www.britannica.com/search?query=" onmouseover="alert(1)</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>ATTR</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>&lt;input name="query" id="search-page-search-query" placeholder="Search Britannica..." class="form-control form-control-lg search-query pr-50 shadow-sm" value="" onmouseover="alert(1)" maxlength="200" autocomplete="off"  aria-label="Search Britannica" /&gt;</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>https://www.britannica.com/search?query=" onmouseover="alert(1)</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>ATTR</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>&lt;input name="query" id="search-page-search-query" placeholder="Search Britannica..." class="form-control form-control-lg search-query pr-50 shadow-sm" value="" onmouseover="alert(1)" maxlength="200" autocomplete="off"  aria-label="Search Britannica" /&gt;</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>https://www.britannica.com/search?query=" onmouseover="alert(1)</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>ATTR</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>&lt;input name="query" id="search-page-search-query" placeholder="Search Britannica..." class="form-control form-control-lg search-query pr-50 shadow-sm" value="" onmouseover="alert(1)" maxlength="200" autocomplete="off"  aria-label="Search Britannica" /&gt;</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>https://www.britannica.com/search?query=" onmouseover="alert(1)</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>ATTR</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>&lt;input name="query" id="search-page-search-query" placeholder="Search Britannica..." class="form-control form-control-lg search-query pr-50 shadow-sm" value="" onmouseover="alert(1)" maxlength="200" autocomplete="off"  aria-label="Search Britannica" /&gt;</t>
-        </is>
+      <c r="D1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>